<commit_message>
添加Excel to PNG的模块， 把Office2PDF以及pdf2img文档整理了形成readme.md，以及reportlab_notes.md和xlrd_notes.md
</commit_message>
<xml_diff>
--- a/res/excel.xlsx
+++ b/res/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huochao\Documents\健康云\业务\肺炎疫情\数据表\中央领导使用表\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zbd\PycharmProjects\mylearn\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E94F177-34AA-4D91-AA2D-F293B149F360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526132E0-CD3F-4B87-8C09-C969259C63B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="690" windowWidth="23385" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="防护服" sheetId="2" r:id="rId1"/>
@@ -630,6 +630,87 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -690,128 +771,47 @@
     <xf numFmtId="58" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1158,16 +1158,16 @@
       <selection activeCell="C9" sqref="C9:O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="3.625" customWidth="1"/>
-    <col min="5" max="9" width="8.5" customWidth="1"/>
-    <col min="10" max="11" width="10.125" customWidth="1"/>
-    <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="13" max="15" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="5" max="9" width="8.44140625" customWidth="1"/>
+    <col min="10" max="11" width="10.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" customWidth="1"/>
+    <col min="13" max="15" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18" customHeight="1">
@@ -1190,161 +1190,161 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="24" customHeight="1">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:18" ht="63" customHeight="1">
+      <c r="A2" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="35">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="62">
         <v>43865</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="34"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:18" ht="26.25" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="31" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="31" t="s">
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="33"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" spans="1:18" ht="26.25" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="57" t="s">
+      <c r="A5" s="68"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="61" t="s">
+      <c r="H5" s="40"/>
+      <c r="I5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="37" t="s">
+      <c r="K5" s="65"/>
+      <c r="L5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="39"/>
-      <c r="N5" s="38"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="65"/>
       <c r="O5" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="26.25" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="63" t="s">
+      <c r="A6" s="68"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="65" t="s">
+      <c r="K6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="65" t="s">
+      <c r="L6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="65" t="s">
+      <c r="M6" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="63" t="s">
+      <c r="O6" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="60"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-    </row>
-    <row r="8" spans="1:18" ht="18.75">
-      <c r="A8" s="42"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+    </row>
+    <row r="8" spans="1:18" ht="17.399999999999999">
+      <c r="A8" s="69"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="55">
+      <c r="C8" s="47">
         <v>1</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="6">
         <v>2</v>
       </c>
@@ -1380,189 +1380,162 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="70" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
       <c r="F9" s="24"/>
       <c r="G9" s="20"/>
       <c r="H9" s="21"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
     </row>
     <row r="10" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A10" s="44"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="20"/>
       <c r="H10" s="21"/>
       <c r="I10" s="24"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="71"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
     </row>
     <row r="11" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A11" s="45"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="20"/>
       <c r="H11" s="21"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
     </row>
     <row r="12" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="70" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="70"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
     </row>
     <row r="13" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A13" s="44"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="23"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="71"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
     </row>
     <row r="14" spans="1:18" ht="29.25" customHeight="1">
-      <c r="A14" s="45"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="23"/>
       <c r="I14" s="22"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
     </row>
     <row r="15" spans="1:18" ht="93.75" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
     </row>
     <row r="16" spans="1:18" ht="25.5" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="O9:O11"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="B4:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
     <mergeCell ref="A15:O15"/>
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="A2:O2"/>
@@ -1579,6 +1552,33 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="B4:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -1595,22 +1595,22 @@
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="7.625" customWidth="1"/>
-    <col min="4" max="4" width="2.875" customWidth="1"/>
-    <col min="5" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" customWidth="1"/>
+    <col min="5" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="9.375" customWidth="1"/>
-    <col min="10" max="10" width="7.75" customWidth="1"/>
-    <col min="11" max="11" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="10.875" customWidth="1"/>
-    <col min="14" max="14" width="10.375" customWidth="1"/>
-    <col min="15" max="15" width="13.875" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1">
@@ -1634,39 +1634,39 @@
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" ht="37.5" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="F3" s="78" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="F3" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="13" t="s">
@@ -1675,75 +1675,75 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:18" ht="33.75" customHeight="1">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="73" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="31" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="33"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" spans="1:18" ht="39.75" customHeight="1">
-      <c r="A5" s="75"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="57" t="s">
+      <c r="A5" s="84"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G5" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="57" t="s">
+      <c r="H5" s="81"/>
+      <c r="I5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="31" t="s">
+      <c r="K5" s="60"/>
+      <c r="L5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="33"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="60"/>
       <c r="O5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="37.5">
-      <c r="A6" s="75"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
+    <row r="6" spans="1:18" ht="34.799999999999997">
+      <c r="A6" s="84"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
       <c r="G6" s="14" t="s">
         <v>30</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="77"/>
+      <c r="I6" s="86"/>
       <c r="J6" s="11" t="s">
         <v>9</v>
       </c>
@@ -1763,13 +1763,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="18.75">
-      <c r="A7" s="76"/>
-      <c r="B7" s="79">
+    <row r="7" spans="1:18" ht="17.399999999999999">
+      <c r="A7" s="85"/>
+      <c r="B7" s="74">
         <v>1</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
       <c r="E7" s="6">
         <v>2</v>
       </c>
@@ -1808,9 +1808,9 @@
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="79"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -1827,9 +1827,9 @@
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -1843,23 +1843,23 @@
       <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:18" ht="98.25" customHeight="1">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
     </row>
     <row r="11" spans="1:18" ht="33.75" customHeight="1">
       <c r="A11" s="4" t="s">
@@ -1882,13 +1882,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B4:D6"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="J4:O4"/>
@@ -1899,6 +1892,13 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B4:D6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>